<commit_message>
Verifies now delegate to validators. Added additional compile-time lint checks. Validations now return new instances if necessary (to support no-op behavior after a fatal validation failure).
</commit_message>
<xml_diff>
--- a/benchmark/benchmark.xlsx
+++ b/benchmark/benchmark.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gili\Documents\requirements\benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gili\Documents\requirements.java\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D62F028-F87C-4319-8675-76207D2F5D6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Benchmark</t>
   </si>
@@ -108,6 +109,72 @@
   </si>
   <si>
     <t>* Size is similar across both releases</t>
+  </si>
+  <si>
+    <t>Major improvement since last version. Overhead less than 1 μs.</t>
+  </si>
+  <si>
+    <t>xBaseline2</t>
+  </si>
+  <si>
+    <t>Slower than previous release but absolute overhead remains low.</t>
+  </si>
+  <si>
+    <t>requireThat() overhead if check passes</t>
+  </si>
+  <si>
+    <t>assertThat() overhead versus invoking requireThat() directly</t>
+  </si>
+  <si>
+    <t>requireThat() check fails, the exception is not caught</t>
+  </si>
+  <si>
+    <t>requireThat() check fails, exception is caught</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>requireThat(java) vs requireThat(guava)</t>
+  </si>
+  <si>
+    <t>JavaTest.requireThat</t>
+  </si>
+  <si>
+    <t>GuavaTest.requireThat</t>
+  </si>
+  <si>
+    <t>JavaTest.assertThatWithAssertionsEnabled</t>
+  </si>
+  <si>
+    <t>JavaTest.requireThatDoesNotContainDuplicates</t>
+  </si>
+  <si>
+    <t>JavaTest.assertThatDoesNotContainDuplicates</t>
+  </si>
+  <si>
+    <t>JavaTest.requireThatThrowException</t>
+  </si>
+  <si>
+    <t>JavaTest.requireThatThrowAndConsumeStackTrace</t>
+  </si>
+  <si>
+    <t>assertThat() overhead versus empty method</t>
+  </si>
+  <si>
+    <t>assertThat() time saved versus doesNotContainDuplicates()</t>
+  </si>
+  <si>
+    <t>JavaTest.requireThatThrowAndConsumeUnmodifiedStackTrace</t>
+  </si>
+  <si>
+    <t>requireThat() check fails, exception is caught, stack trace is not cleaned</t>
+  </si>
+  <si>
+    <t>9cb02049f7a5d7a6d839955bb47b4e55e3505ab7</t>
+  </si>
+  <si>
+    <t>* Absolute performance overhead is under 10 µs</t>
   </si>
   <si>
     <r>
@@ -129,83 +196,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Microsoft Windows [Version 10.0.17763.348], 64-bit, JDK 12-ea+33, Antivirus disabled</t>
+      <t xml:space="preserve"> Microsoft Windows [Version 10.0.18362.207], 64-bit, JDK 12.0.1, Antivirus disabled</t>
     </r>
   </si>
   <si>
-    <t>Major improvement since last version. Overhead less than 1 μs.</t>
-  </si>
-  <si>
-    <t>xBaseline2</t>
-  </si>
-  <si>
-    <t>Slower than previous release but absolute overhead remains low.</t>
-  </si>
-  <si>
-    <t>requireThat() overhead if check passes</t>
-  </si>
-  <si>
-    <t>assertThat() overhead versus invoking requireThat() directly</t>
-  </si>
-  <si>
-    <t>requireThat() check fails, the exception is not caught</t>
-  </si>
-  <si>
-    <t>requireThat() check fails, exception is caught</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>requireThat(java) vs requireThat(guava)</t>
-  </si>
-  <si>
-    <t>JavaTest.requireThat</t>
-  </si>
-  <si>
-    <t>GuavaTest.requireThat</t>
-  </si>
-  <si>
-    <t>JavaTest.assertThatWithAssertionsEnabled</t>
-  </si>
-  <si>
-    <t>JavaTest.requireThatDoesNotContainDuplicates</t>
-  </si>
-  <si>
-    <t>JavaTest.assertThatDoesNotContainDuplicates</t>
-  </si>
-  <si>
-    <t>JavaTest.requireThatThrowException</t>
-  </si>
-  <si>
-    <t>JavaTest.requireThatThrowAndConsumeStackTrace</t>
-  </si>
-  <si>
-    <t>assertThat() overhead versus empty method</t>
-  </si>
-  <si>
-    <t>assertThat() time saved versus doesNotContainDuplicates()</t>
-  </si>
-  <si>
-    <t>JavaTest.requireThatThrowAndConsumeUnmodifiedStackTrace</t>
-  </si>
-  <si>
-    <t>requireThat() check fails, exception is caught, stack trace is not cleaned</t>
-  </si>
-  <si>
-    <t>9cb02049f7a5d7a6d839955bb47b4e55e3505ab7</t>
-  </si>
-  <si>
-    <t>8fa3c1b91dad5974e789db7885a2d04051d221f7</t>
-  </si>
-  <si>
-    <t>* Absolute performance overhead is under 10 µs</t>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>25a18f00474bb60a560825f4e198db44d1803875</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
@@ -506,60 +510,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A37:D42" totalsRowShown="0">
-  <autoFilter ref="A37:D42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A37:D42" totalsRowShown="0">
+  <autoFilter ref="A37:D42" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Artifact"/>
-    <tableColumn id="2" name="4.0.4-RC" dataDxfId="15"/>
-    <tableColumn id="6" name="4.0.6-RC" dataDxfId="14"/>
-    <tableColumn id="7" name="% Change" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Artifact"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="4.0.4-RC" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="4.0.6-RC" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="% Change" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:K18" totalsRowShown="0">
-  <autoFilter ref="A7:K18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A7:K18" totalsRowShown="0">
+  <autoFilter ref="A7:K18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="3" name="Benchmark"/>
-    <tableColumn id="4" name="Nanoseconds" dataDxfId="12"/>
-    <tableColumn id="5" name="Error" dataDxfId="11"/>
-    <tableColumn id="14" name="% Error" dataDxfId="10"/>
-    <tableColumn id="6" name="xBaseline" dataDxfId="9"/>
-    <tableColumn id="22" name="Nanoseconds2" dataDxfId="8"/>
-    <tableColumn id="23" name="Error2" dataDxfId="7"/>
-    <tableColumn id="24" name="% Error2" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Benchmark"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Nanoseconds" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Error" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="% Error" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="xBaseline" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Nanoseconds2" dataDxfId="8"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Error2" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="% Error2" dataDxfId="6">
       <calculatedColumnFormula>#REF!/#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="xBaseline2" dataDxfId="5" dataCellStyle="Neutral"/>
-    <tableColumn id="26" name="% Change2" dataDxfId="4" dataCellStyle="Neutral">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="xBaseline2" dataDxfId="5" dataCellStyle="Neutral"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="% Change2" dataDxfId="4" dataCellStyle="Neutral">
       <calculatedColumnFormula>#REF!/#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Comment" dataDxfId="3" dataCellStyle="Neutral"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Comment" dataDxfId="3" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:B4" totalsRowShown="0">
-  <autoFilter ref="A2:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A2:B4" totalsRowShown="0">
+  <autoFilter ref="A2:B4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Version"/>
-    <tableColumn id="2" name="Changeset"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Version"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Changeset"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A22:C30" totalsRowShown="0">
-  <autoFilter ref="A22:C30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A22:C30" totalsRowShown="0">
+  <autoFilter ref="A22:C30" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Description" dataDxfId="2"/>
-    <tableColumn id="2" name="Nanoseconds" dataDxfId="1"/>
-    <tableColumn id="4" name="Nanoseconds2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Nanoseconds" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Nanoseconds2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -827,10 +831,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -850,7 +856,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -863,18 +869,18 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -914,7 +920,7 @@
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -957,7 +963,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1">
         <v>10.234999999999999</v>
@@ -986,12 +992,12 @@
         <v>1.3751831949193942</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>16.228999999999999</v>
@@ -1026,12 +1032,12 @@
         <v>1.3704479635220901</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1">
         <v>37.865000000000002</v>
@@ -1066,12 +1072,12 @@
         <v>1.247748580483296</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1">
         <v>2245.5880000000002</v>
@@ -1101,7 +1107,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1">
         <v>6.25</v>
@@ -1132,7 +1138,7 @@
         <v>1.9676800000000001</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1169,7 +1175,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1">
         <v>44562.173999999999</v>
@@ -1204,7 +1210,7 @@
         <v>4.4408448295184158E-2</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1241,7 +1247,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1">
         <v>56395.707000000002</v>
@@ -1279,7 +1285,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1">
         <v>55572.826999999997</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -1361,7 +1367,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
         <f>B9-B8</f>
@@ -1380,7 +1386,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1">
         <f>B10-B9</f>
@@ -1399,7 +1405,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <f>B11-B9</f>
@@ -1418,7 +1424,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1">
         <f>B13-B8</f>
@@ -1437,7 +1443,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="22">
         <f>B12-B13</f>
@@ -1456,7 +1462,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="21">
         <f>B15-B14</f>
@@ -1475,7 +1481,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1">
         <f>B17-B16</f>
@@ -1494,7 +1500,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="21">
         <f>B18-B16</f>
@@ -1661,7 +1667,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:8">

</xml_diff>

<commit_message>
Updated benchmarks for 5.1.2
</commit_message>
<xml_diff>
--- a/benchmark/benchmark.xlsx
+++ b/benchmark/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gili\Documents\requirements.java\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0031E5B1-7586-4188-92F4-94E0AC78D7D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9C5407-90CD-4944-9F25-45DFEB2571FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Benchmark</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Changeset</t>
   </si>
   <si>
-    <t>4.0.6-RC</t>
-  </si>
-  <si>
     <t>Version:</t>
   </si>
   <si>
@@ -105,7 +102,82 @@
     <t>assertThat() overhead versus empty method</t>
   </si>
   <si>
-    <t>9cb02049f7a5d7a6d839955bb47b4e55e3505ab7</t>
+    <t>Order reported by JMH</t>
+  </si>
+  <si>
+    <t>Order for improved readability</t>
+  </si>
+  <si>
+    <t>Reasonable overhead for uncommon execution path</t>
+  </si>
+  <si>
+    <t>GcTest.assertThatWithAssertionsDisabled</t>
+  </si>
+  <si>
+    <t>GcTest.emptyMethod</t>
+  </si>
+  <si>
+    <t>GcTest.requireThat</t>
+  </si>
+  <si>
+    <t>Alloc rate (bytes / operation)</t>
+  </si>
+  <si>
+    <t>%Overhead</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>Alloc error</t>
+  </si>
+  <si>
+    <t>Alloc rate</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Absolute overhead remains low</t>
+  </si>
+  <si>
+    <t>assertThat() time saved versus requireThat()</t>
+  </si>
+  <si>
+    <t>ExceptionTest.throwAndConsumeStackTrace</t>
+  </si>
+  <si>
+    <t>ExceptionTest.requireThatThrowException</t>
+  </si>
+  <si>
+    <t>ExceptionTest.throwException</t>
+  </si>
+  <si>
+    <t>GcTest.assertThatWithAssertionsEnabled</t>
+  </si>
+  <si>
+    <t>5.1.0</t>
+  </si>
+  <si>
+    <t>ExceptionTest.requireThatThrowAndConsumeStackTrace</t>
+  </si>
+  <si>
+    <t>requireThat() check fails, the stack trace is not consumed</t>
+  </si>
+  <si>
+    <t>requireThat() check fails, the stack trace is consumed</t>
+  </si>
+  <si>
+    <t>a8908e65c2cc9d49d43ea5a1a3277ff7aa4aee77</t>
+  </si>
+  <si>
+    <t>5.1.2</t>
+  </si>
+  <si>
+    <t>45db46a6557b1aa3d7aec4319fb21c1a932a6830</t>
+  </si>
+  <si>
+    <t>* Absolute performance overhead for the common execution path is under 10 µs</t>
   </si>
   <si>
     <r>
@@ -127,86 +199,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Microsoft Windows [Version 10.0.18362.207], 64-bit, JDK 12.0.1, Antivirus disabled</t>
+      <t xml:space="preserve"> Microsoft Windows [Version 10.0.18362.267], 64-bit, JDK 12.0.1, Antivirus disabled</t>
     </r>
-  </si>
-  <si>
-    <t>Order reported by JMH</t>
-  </si>
-  <si>
-    <t>Order for improved readability</t>
-  </si>
-  <si>
-    <t>Reasonable overhead for uncommon execution path</t>
-  </si>
-  <si>
-    <t>GcTest.assertThatWithAssertionsDisabled</t>
-  </si>
-  <si>
-    <t>GcTest.emptyMethod</t>
-  </si>
-  <si>
-    <t>GcTest.requireThat</t>
-  </si>
-  <si>
-    <t>Alloc rate (bytes / operation)</t>
-  </si>
-  <si>
-    <t>%Overhead</t>
-  </si>
-  <si>
-    <t>Overhead</t>
-  </si>
-  <si>
-    <t>Alloc error</t>
-  </si>
-  <si>
-    <t>Alloc rate</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Absolute overhead remains low</t>
-  </si>
-  <si>
-    <t>Benchmarks changed so comparison is not meaningful</t>
-  </si>
-  <si>
-    <t>assertThat() time saved versus requireThat()</t>
-  </si>
-  <si>
-    <t>* validateThat() functionality increased JAR size by 42%</t>
-  </si>
-  <si>
-    <t>ExceptionTest.throwAndConsumeStackTrace</t>
-  </si>
-  <si>
-    <t>ExceptionTest.requireThatThrowException</t>
-  </si>
-  <si>
-    <t>ExceptionTest.throwException</t>
-  </si>
-  <si>
-    <t>GcTest.assertThatWithAssertionsEnabled</t>
-  </si>
-  <si>
-    <t>5.1.0</t>
-  </si>
-  <si>
-    <t>ExceptionTest.requireThatThrowAndConsumeStackTrace</t>
-  </si>
-  <si>
-    <t>requireThat() check fails, the stack trace is not consumed</t>
-  </si>
-  <si>
-    <t>requireThat() check fails, the stack trace is consumed</t>
-  </si>
-  <si>
-    <t>* Absolute performance overhead for the common execution path is under 15 µs</t>
-  </si>
-  <si>
-    <t>a8908e65c2cc9d49d43ea5a1a3277ff7aa4aee77</t>
   </si>
 </sst>
 </file>
@@ -312,7 +306,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -334,7 +328,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -593,9 +586,9 @@
   <autoFilter ref="A46:D51" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Artifact"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="4.0.6-RC" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="5.1.0" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="% Change" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="5.1.0" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="5.1.2" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="% Change" dataDxfId="18" dataCellStyle="Good"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -929,7 +922,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -949,7 +942,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -962,10 +955,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>26</v>
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -973,17 +966,17 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="16"/>
     </row>
@@ -998,156 +991,156 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B9" s="12">
-        <v>76290.758000000002</v>
+        <v>73249.623000000007</v>
       </c>
       <c r="C9" s="12">
-        <v>1225.5450000000001</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+        <v>1341.943</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" s="12">
-        <v>2620.8049999999998</v>
+        <v>2613.6640000000002</v>
       </c>
       <c r="C10" s="12">
-        <v>65.349999999999994</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+        <v>34.201000000000001</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B11" s="12">
-        <v>62485.987000000001</v>
+        <v>63727.654000000002</v>
       </c>
       <c r="C11" s="12">
-        <v>752.33199999999999</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+        <v>916.64599999999996</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" s="12">
-        <v>1669.713</v>
+        <v>1716.7329999999999</v>
       </c>
       <c r="C12" s="12">
-        <v>28.37</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+        <v>24.527000000000001</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="12">
-        <v>5.7450000000000001</v>
+        <v>5.2830000000000004</v>
       </c>
       <c r="C13" s="12">
-        <v>0.193</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D13" s="12">
         <v>0</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>39</v>
+      <c r="E13" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B14" s="12">
-        <v>129.96899999999999</v>
+        <v>130.50399999999999</v>
       </c>
       <c r="C14" s="12">
-        <v>1.681</v>
+        <v>1.111</v>
       </c>
       <c r="D14" s="12">
-        <v>216.392</v>
+        <v>1502.0229999999999</v>
       </c>
       <c r="E14" s="12">
-        <v>0.46200000000000002</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="12">
-        <v>0.87</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="C15" s="12">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>39</v>
+      <c r="E15" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="12">
-        <v>115.071</v>
+        <v>121.38800000000001</v>
       </c>
       <c r="C16" s="12">
-        <v>1.137</v>
+        <v>1.0660000000000001</v>
       </c>
       <c r="D16" s="12">
-        <v>216.446</v>
+        <v>216</v>
       </c>
       <c r="E16" s="12">
-        <v>0.47299999999999998</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="12">
-        <v>118.401</v>
+        <v>122.46299999999999</v>
       </c>
       <c r="C17" s="12">
-        <v>0.85499999999999998</v>
+        <v>1.1479999999999999</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>48</v>
@@ -1170,19 +1163,19 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H21" t="s">
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K21" t="s">
         <v>12</v>
@@ -1193,107 +1186,104 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" s="17">
-        <v>0.88300000000000001</v>
+        <v>0.87</v>
       </c>
       <c r="C22" s="17">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D22" s="17">
         <f t="shared" ref="D22:G23" si="0">B15</f>
-        <v>0.87</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="E22" s="17">
         <f t="shared" si="0"/>
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F22" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="26" t="str">
+      <c r="G22" s="25" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
       <c r="H22" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>6.8965517241379309E-3</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>39</v>
+        <v>8.5836909871244635E-3</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="K22" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>0.98527746319365794</v>
+        <v>1.071264367816092</v>
       </c>
       <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
-        <v>16.298999999999999</v>
+        <v>115.071</v>
       </c>
       <c r="C23" s="1">
-        <v>0.11600000000000001</v>
+        <v>1.137</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>115.071</v>
+        <v>121.38800000000001</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>1.137</v>
+        <v>1.0660000000000001</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>216.446</v>
+        <v>216</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
-        <v>0.47299999999999998</v>
+        <v>1E-3</v>
       </c>
       <c r="H23" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>9.8808561670620746E-3</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>39</v>
+        <v>8.7817576696213803E-3</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="K23" s="11">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>7.0600036812074363</v>
-      </c>
-      <c r="L23" t="s">
-        <v>41</v>
+        <v>1.054896542134856</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>23.277000000000001</v>
+        <v>118.401</v>
       </c>
       <c r="C24" s="1">
-        <v>0.21199999999999999</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="D24" s="1">
         <f>B17</f>
-        <v>118.401</v>
+        <v>122.46299999999999</v>
       </c>
       <c r="E24" s="1">
         <f>C17</f>
-        <v>0.85499999999999998</v>
+        <v>1.1479999999999999</v>
       </c>
       <c r="F24" s="1">
         <f>D17</f>
@@ -1305,266 +1295,260 @@
       </c>
       <c r="H24" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>7.2212227937264043E-3</v>
+        <v>9.3742599805655587E-3</v>
       </c>
       <c r="I24" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/D23</f>
-        <v>1.0289386552650104</v>
-      </c>
-      <c r="J24" s="22">
+        <v>1.0088559000889707</v>
+      </c>
+      <c r="J24" s="21">
         <f>Table1[[#This Row],[Nanoseconds2]]-D23</f>
-        <v>3.3299999999999983</v>
-      </c>
-      <c r="K24" s="11">
+        <v>1.0749999999999886</v>
+      </c>
+      <c r="K24" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>5.08660909911071</v>
-      </c>
-      <c r="L24" t="s">
-        <v>41</v>
+        <v>1.0343071426761599</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1">
-        <v>54.615000000000002</v>
+        <v>129.96899999999999</v>
       </c>
       <c r="C25" s="1">
-        <v>0.32700000000000001</v>
+        <v>1.681</v>
       </c>
       <c r="D25" s="1">
         <f>B14</f>
-        <v>129.96899999999999</v>
+        <v>130.50399999999999</v>
       </c>
       <c r="E25" s="1">
         <f>C14</f>
-        <v>1.681</v>
+        <v>1.111</v>
       </c>
       <c r="F25" s="1">
         <f>D14</f>
-        <v>216.392</v>
+        <v>1502.0229999999999</v>
       </c>
       <c r="G25" s="1">
         <f>E14</f>
-        <v>0.46200000000000002</v>
+        <v>12.77</v>
       </c>
       <c r="H25" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>1.293385345736291E-2</v>
+        <v>8.5131490222521925E-3</v>
       </c>
       <c r="I25" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/D23</f>
-        <v>1.1294678937351721</v>
-      </c>
-      <c r="J25" s="20">
+        <v>1.0750980327544732</v>
+      </c>
+      <c r="J25" s="19">
         <f>Table1[[#This Row],[Nanoseconds2]]-D23</f>
-        <v>14.897999999999996</v>
-      </c>
-      <c r="K25" s="11">
+        <v>9.1159999999999854</v>
+      </c>
+      <c r="K25" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>2.3797308431749515</v>
-      </c>
-      <c r="L25" t="s">
-        <v>41</v>
+        <v>1.004116366210404</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1">
-        <v>14.531000000000001</v>
+        <v>5.7450000000000001</v>
       </c>
       <c r="C26" s="1">
-        <v>0.121</v>
+        <v>0.193</v>
       </c>
       <c r="D26" s="1">
         <f>B13</f>
-        <v>5.7450000000000001</v>
+        <v>5.2830000000000004</v>
       </c>
       <c r="E26" s="1">
         <f>C13</f>
-        <v>0.193</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="F26" s="1">
         <f>D13</f>
         <v>0</v>
       </c>
-      <c r="G26" s="25" t="str">
+      <c r="G26" s="24" t="str">
         <f>E13</f>
         <v>N/A</v>
       </c>
       <c r="H26" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>3.3594429939077457E-2</v>
+        <v>1.1167897028203672E-2</v>
       </c>
       <c r="I26" s="5">
         <f>Table1[[#This Row],[Nanoseconds2]]/D22</f>
-        <v>6.6034482758620694</v>
-      </c>
-      <c r="J26" s="20">
+        <v>5.6684549356223179</v>
+      </c>
+      <c r="J26" s="19">
         <f>Table1[[#This Row],[Nanoseconds2]]-D22</f>
-        <v>4.875</v>
+        <v>4.351</v>
       </c>
       <c r="K26" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>0.39536164063037643</v>
+        <v>0.91958224543080946</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1">
-        <v>1624.385</v>
+        <v>1669.713</v>
       </c>
       <c r="C27" s="1">
-        <v>22.85</v>
+        <v>28.37</v>
       </c>
       <c r="D27" s="1">
         <f>B12</f>
-        <v>1669.713</v>
+        <v>1716.7329999999999</v>
       </c>
       <c r="E27" s="1">
         <f>C12</f>
-        <v>28.37</v>
+        <v>24.527000000000001</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>1.6990943952643358E-2</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>39</v>
+        <v>1.4287020753955333E-2</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="K27" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>1.0279047147074123</v>
+        <v>1.0281605281865807</v>
       </c>
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1">
-        <v>2402.1219999999998</v>
+        <v>2620.8049999999998</v>
       </c>
       <c r="C28" s="1">
-        <v>53.872999999999998</v>
+        <v>65.349999999999994</v>
       </c>
       <c r="D28" s="1">
         <f>B10</f>
-        <v>2620.8049999999998</v>
+        <v>2613.6640000000002</v>
       </c>
       <c r="E28" s="1">
         <f>C10</f>
-        <v>65.349999999999994</v>
+        <v>34.201000000000001</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>2.4935086738616569E-2</v>
+        <v>1.3085461635466531E-2</v>
       </c>
       <c r="I28" s="11">
         <f>Table1[[#This Row],[Nanoseconds2]]/D27</f>
-        <v>1.5696140594221881</v>
-      </c>
-      <c r="J28" s="23">
+        <v>1.5224638892594249</v>
+      </c>
+      <c r="J28" s="22">
         <f>Table1[[#This Row],[Nanoseconds2]]-D27</f>
-        <v>951.09199999999987</v>
-      </c>
-      <c r="K28" s="11">
+        <v>896.93100000000027</v>
+      </c>
+      <c r="K28" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>1.0910374244105836</v>
+        <v>0.99727526466104899</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1">
-        <v>60593.071000000004</v>
+        <v>62485.987000000001</v>
       </c>
       <c r="C29" s="1">
-        <v>743.47299999999996</v>
+        <v>752.33199999999999</v>
       </c>
       <c r="D29" s="1">
         <f>B11</f>
-        <v>62485.987000000001</v>
+        <v>63727.654000000002</v>
       </c>
       <c r="E29" s="1">
         <f>C11</f>
-        <v>752.33199999999999</v>
+        <v>916.64599999999996</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>1.2040011466890968E-2</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>39</v>
+        <v>1.4383802673796841E-2</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="K29" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>1.0312398095815278</v>
+        <v>1.0198711272657019</v>
       </c>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1">
-        <v>68267.453999999998</v>
+        <v>76290.758000000002</v>
       </c>
       <c r="C30" s="1">
-        <v>894.97699999999998</v>
+        <v>1225.5450000000001</v>
       </c>
       <c r="D30" s="1">
         <f>B9</f>
-        <v>76290.758000000002</v>
+        <v>73249.623000000007</v>
       </c>
       <c r="E30" s="1">
         <f>C9</f>
-        <v>1225.5450000000001</v>
+        <v>1341.943</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="10">
         <f>Table1[[#This Row],[Error2]]/Table1[[#This Row],[Nanoseconds2]]</f>
-        <v>1.6064134531210191E-2</v>
+        <v>1.8320135244928152E-2</v>
       </c>
       <c r="I30" s="11">
         <f>Table1[[#This Row],[Nanoseconds2]]/D29</f>
-        <v>1.2209258693473146</v>
-      </c>
-      <c r="J30" s="23">
+        <v>1.1494165939326748</v>
+      </c>
+      <c r="J30" s="22">
         <f>Table1[[#This Row],[Nanoseconds2]]-D29</f>
-        <v>13804.771000000001</v>
-      </c>
-      <c r="K30" s="11">
+        <v>9521.9690000000046</v>
+      </c>
+      <c r="K30" s="4">
         <f>Table1[[#This Row],[Nanoseconds2]]/Table1[[#This Row],[Nanoseconds]]</f>
-        <v>1.1175275117188346</v>
+        <v>0.96013757000553079</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1599,7 +1583,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>1</v>
@@ -1616,15 +1600,15 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="1">
         <f>B23-B22</f>
-        <v>15.416</v>
+        <v>114.20099999999999</v>
       </c>
       <c r="C35" s="1">
         <f>D23-D22</f>
-        <v>114.20099999999999</v>
+        <v>120.456</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="3"/>
@@ -1635,15 +1619,15 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1">
         <f>B24-B23</f>
-        <v>6.9780000000000015</v>
-      </c>
-      <c r="C36" s="20">
+        <v>3.3299999999999983</v>
+      </c>
+      <c r="C36" s="19">
         <f>D24-D23</f>
-        <v>3.3299999999999983</v>
+        <v>1.0749999999999886</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="3"/>
@@ -1654,15 +1638,15 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B37" s="1">
         <f>B25-B23</f>
-        <v>38.316000000000003</v>
-      </c>
-      <c r="C37" s="23">
+        <v>14.897999999999996</v>
+      </c>
+      <c r="C37" s="19">
         <f>D25-D23</f>
-        <v>14.897999999999996</v>
+        <v>9.1159999999999854</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="3"/>
@@ -1673,15 +1657,15 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1">
         <f>B26-B22</f>
-        <v>13.648</v>
-      </c>
-      <c r="C38" s="20">
+        <v>4.875</v>
+      </c>
+      <c r="C38" s="19">
         <f>D26-D22</f>
-        <v>4.875</v>
+        <v>4.351</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="3"/>
@@ -1692,15 +1676,15 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="20">
+        <v>38</v>
+      </c>
+      <c r="B39" s="19">
         <f>B24-B26</f>
-        <v>8.7460000000000004</v>
-      </c>
-      <c r="C39" s="20">
+        <v>112.65599999999999</v>
+      </c>
+      <c r="C39" s="19">
         <f>D23-D26</f>
-        <v>109.32599999999999</v>
+        <v>116.105</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="3"/>
@@ -1711,15 +1695,15 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B40" s="19">
         <f>B28-B27</f>
-        <v>777.73699999999985</v>
-      </c>
-      <c r="C40" s="20">
+        <v>951.09199999999987</v>
+      </c>
+      <c r="C40" s="19">
         <f>D28-D27</f>
-        <v>951.09199999999987</v>
+        <v>896.93100000000027</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="3"/>
@@ -1730,15 +1714,15 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1">
         <f>B30-B29</f>
-        <v>7674.3829999999944</v>
+        <v>13804.771000000001</v>
       </c>
       <c r="C41" s="1">
         <f>D30-D29</f>
-        <v>13804.771000000001</v>
+        <v>9521.9690000000046</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="3"/>
@@ -1787,7 +1771,7 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
@@ -1801,14 +1785,14 @@
         <v>8</v>
       </c>
       <c r="B47" s="2">
-        <v>203370</v>
+        <v>299573</v>
       </c>
       <c r="C47" s="2">
-        <v>299573</v>
-      </c>
-      <c r="D47" s="11">
-        <f>Table2[[#This Row],[5.1.0]]/Table2[[#This Row],[4.0.6-RC]]</f>
-        <v>1.4730442051433348</v>
+        <v>300439</v>
+      </c>
+      <c r="D47" s="4">
+        <f>Table2[[#This Row],[5.1.2]]/Table2[[#This Row],[5.1.0]]</f>
+        <v>1.002890781211925</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1816,14 +1800,14 @@
         <v>3</v>
       </c>
       <c r="B48" s="2">
-        <v>11911</v>
+        <v>18833</v>
       </c>
       <c r="C48" s="2">
-        <v>18833</v>
+        <v>18843</v>
       </c>
       <c r="D48" s="4">
-        <f>Table2[[#This Row],[5.1.0]]/Table2[[#This Row],[4.0.6-RC]]</f>
-        <v>1.5811434808160525</v>
+        <f>Table2[[#This Row],[5.1.2]]/Table2[[#This Row],[5.1.0]]</f>
+        <v>1.0005309828492539</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1831,14 +1815,14 @@
         <v>14</v>
       </c>
       <c r="B49" s="2">
-        <v>17028</v>
+        <v>18001</v>
       </c>
       <c r="C49" s="2">
-        <v>18001</v>
+        <v>17917</v>
       </c>
       <c r="D49" s="4">
-        <f>Table2[[#This Row],[5.1.0]]/Table2[[#This Row],[4.0.6-RC]]</f>
-        <v>1.0571411792342025</v>
+        <f>Table2[[#This Row],[5.1.2]]/Table2[[#This Row],[5.1.0]]</f>
+        <v>0.9953335925781901</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1846,14 +1830,14 @@
         <v>4</v>
       </c>
       <c r="B50" s="2">
-        <v>13603</v>
+        <v>12930</v>
       </c>
       <c r="C50" s="2">
-        <v>12930</v>
+        <v>12906</v>
       </c>
       <c r="D50" s="4">
-        <f>Table2[[#This Row],[5.1.0]]/Table2[[#This Row],[4.0.6-RC]]</f>
-        <v>0.95052561934867308</v>
+        <f>Table2[[#This Row],[5.1.2]]/Table2[[#This Row],[5.1.0]]</f>
+        <v>0.99814385150812068</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1862,15 +1846,15 @@
       </c>
       <c r="B51" s="9">
         <f>SUM(B47:B50)</f>
-        <v>245912</v>
+        <v>349337</v>
       </c>
       <c r="C51" s="9">
         <f>SUM(C47:C50)</f>
-        <v>349337</v>
-      </c>
-      <c r="D51" s="11">
-        <f>Table2[[#This Row],[5.1.0]]/Table2[[#This Row],[4.0.6-RC]]</f>
-        <v>1.4205772796772829</v>
+        <v>350105</v>
+      </c>
+      <c r="D51" s="4">
+        <f>Table2[[#This Row],[5.1.2]]/Table2[[#This Row],[5.1.0]]</f>
+        <v>1.0021984502071066</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1880,12 +1864,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:1">

</xml_diff>

<commit_message>
* Renamed assumeThat() to that(). Users are expected to invoke "assert that()" * Removed all public references to the validator configuration and the ability to create custom validator factories. * Renamed Configuration.lazyExceptions to recordStacktrace. * Use normal StampedLock because we don't actually need a reentrant lock.
</commit_message>
<xml_diff>
--- a/benchmark/benchmark.xlsx
+++ b/benchmark/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gili\Documents\requirements.java\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A72BFFF-D42C-4C7E-92CC-E91D4FC9D177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946FE18D-4C0C-4D80-B31A-1070E7CA4B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9.0.0" sheetId="1" r:id="rId1"/>
@@ -1159,7 +1159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B62B9BB-0576-4C33-810A-EDE6181CAAFA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>